<commit_message>
Appended graph to output.xlsx
Also removed unncessary print functions
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -577,6 +577,1868 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Simulation Results</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>output!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> Avg. Time in System</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>output!$A$2:$A$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>output!$C$2:$C$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>370.65321699999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>205.514038</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>121.540266</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>105.22588</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>91.189145999999994</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>82.258853000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>69.263817000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>69.397396000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>64.496313000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>60.875202999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>57.067852000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>54.835653000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>54.369852999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>51.761862999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>48.771624000000003</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>48.866000999999997</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>45.976466000000002</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>48.053075999999997</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>45.547832999999997</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>45.935890999999998</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>45.296711999999999</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>44.248787</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>42.042565000000003</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>41.482624000000001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>42.760066999999999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>41.737088</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>41.296733000000003</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>42.637303000000003</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>40.131887999999996</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>40.480255</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>40.565703999999997</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>38.634649000000003</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>39.365125999999997</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>39.482691000000003</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>38.058045999999997</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>37.906109999999998</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>39.605510000000002</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>36.398558999999999</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>38.64855</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>38.123122000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4C37-4921-8891-CE8B856F59FE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>output!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Avg. Time in Queue</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>output!$A$2:$A$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>output!$D$2:$D$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>340.37555800000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>175.51321999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>91.586129</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>75.384651000000005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>61.057253000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>52.16404</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>39.472859999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>38.851505000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>34.307924999999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>31.232081999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>27.453512</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>24.757075</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>24.340789000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>21.634212999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>19.171447000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>18.739671000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16.160561999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17.906783000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>16.007193999999998</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>15.445363</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>15.090833</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>14.224907</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>12.291589</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>11.887382000000001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12.365902999999999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>11.72273</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>11.091597</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>12.119026</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>10.406442999999999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>10.170502000000001</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>9.7791599999999992</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>8.7457499999999992</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>9.223732</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>9.1029839999999993</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8.0256749999999997</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>7.6123570000000003</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9.3736510000000006</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>6.9628240000000003</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>8.2557969999999994</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>7.9345850000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4C37-4921-8891-CE8B856F59FE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>output!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Theoretical Time in Queue</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>output!$A$2:$A$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>output!$E$2:$E$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42.857143000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>37.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>33.333333000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>27.272727</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>23.076923000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>21.428571000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>18.75</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17.647058999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>16.666667</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>15.789474</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>14.285714</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>13.636364</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>13.043478</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>11.538462000000001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>11.111110999999999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>10.714286</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>10.344828</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>9.6774190000000004</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>9.375</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>9.0909089999999999</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>8.8235290000000006</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8.5714290000000002</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>8.3333329999999997</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>8.1081079999999996</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>7.8947370000000001</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>7.6923079999999997</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>7.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-4C37-4921-8891-CE8B856F59FE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="427844504"/>
+        <c:axId val="427845816"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="427844504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="51"/>
+          <c:min val="10"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Interarrival Times</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="427845816"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="427845816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time (Units)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="427844504"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -876,9 +2738,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S14" sqref="S14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1579,5 +3450,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>